<commit_message>
fixed hetero atoms in compounds properties
</commit_message>
<xml_diff>
--- a/example/data/calibration.xlsx
+++ b/example/data/calibration.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/gcms_data_analysis/example/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/gcms_data_analysis/tests/data_for_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{80D8D431-E6ED-47F4-880D-792C42C77B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2998DAD9-3821-4C20-92F6-6655F35D7E24}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{80D8D431-E6ED-47F4-880D-792C42C77B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{219979A2-1E4C-44CD-A67C-652881EF5D40}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6D821E06-881F-4115-BBEA-B9244CF9E454}"/>
+    <workbookView xWindow="13410" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{6D821E06-881F-4115-BBEA-B9244CF9E454}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Calibration!$A$2:$N$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Calibration!$A$2:$N$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>MW</t>
   </si>
@@ -102,19 +102,27 @@
   </si>
   <si>
     <t>(9Z,12Z)-octadeca-9,12-dienoic acid</t>
+  </si>
+  <si>
+    <t>2,4,5-trichlorophenol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,11 +175,47 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -481,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A882931E-0B21-4C7C-B3C2-8F125F51A6CC}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="A4" sqref="A4:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -633,55 +677,55 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="7">
-        <v>228.37090000000001</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9">
+        <v>197.4</v>
+      </c>
+      <c r="C4" s="10">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10">
         <v>10</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="10">
         <v>20</v>
       </c>
-      <c r="E4" s="4">
-        <v>35</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="F4" s="10">
         <v>50</v>
       </c>
-      <c r="G4" s="4">
-        <v>100</v>
-      </c>
-      <c r="H4" s="5">
-        <v>300</v>
-      </c>
-      <c r="I4" s="4">
-        <v>70675</v>
-      </c>
-      <c r="J4" s="6">
-        <v>203215</v>
-      </c>
-      <c r="K4" s="6">
-        <v>500430</v>
-      </c>
-      <c r="L4" s="6">
-        <v>469543</v>
-      </c>
-      <c r="M4" s="4">
-        <v>2957268</v>
-      </c>
-      <c r="N4" s="6">
-        <v>11730886</v>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="12">
+        <v>155710</v>
+      </c>
+      <c r="J4" s="12">
+        <v>343277</v>
+      </c>
+      <c r="K4" s="12">
+        <v>805095</v>
+      </c>
+      <c r="L4" s="12">
+        <v>2302730</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7">
-        <v>256.42410000000001</v>
+        <v>228.37090000000001</v>
       </c>
       <c r="C5" s="4">
         <v>10</v>
@@ -702,33 +746,33 @@
         <v>300</v>
       </c>
       <c r="I5" s="4">
-        <v>51545</v>
+        <v>70675</v>
       </c>
       <c r="J5" s="6">
-        <v>130834</v>
+        <v>203215</v>
       </c>
       <c r="K5" s="6">
-        <v>361070</v>
+        <v>500430</v>
       </c>
       <c r="L5" s="6">
-        <v>430809</v>
+        <v>469543</v>
       </c>
       <c r="M5" s="4">
-        <v>3164919</v>
-      </c>
-      <c r="N5" s="4">
-        <v>12451729</v>
+        <v>2957268</v>
+      </c>
+      <c r="N5" s="6">
+        <v>11730886</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="7">
-        <v>280.44549999999998</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>256.42410000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10</v>
       </c>
       <c r="D6" s="4">
         <v>20</v>
@@ -736,8 +780,8 @@
       <c r="E6" s="4">
         <v>35</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
+      <c r="F6" s="4">
+        <v>50</v>
       </c>
       <c r="G6" s="4">
         <v>100</v>
@@ -745,34 +789,34 @@
       <c r="H6" s="5">
         <v>300</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>18</v>
+      <c r="I6" s="4">
+        <v>51545</v>
       </c>
       <c r="J6" s="6">
-        <v>22338</v>
+        <v>130834</v>
       </c>
       <c r="K6" s="6">
-        <v>63841</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>18</v>
+        <v>361070</v>
+      </c>
+      <c r="L6" s="6">
+        <v>430809</v>
       </c>
       <c r="M6" s="4">
-        <v>741540</v>
+        <v>3164919</v>
       </c>
       <c r="N6" s="4">
-        <v>3975200</v>
+        <v>12451729</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
-        <v>282.46140000000003</v>
-      </c>
-      <c r="C7" s="4">
-        <v>10</v>
+        <v>280.44549999999998</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="4">
         <v>20</v>
@@ -780,8 +824,8 @@
       <c r="E7" s="4">
         <v>35</v>
       </c>
-      <c r="F7" s="4">
-        <v>50</v>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="G7" s="4">
         <v>100</v>
@@ -789,22 +833,66 @@
       <c r="H7" s="5">
         <v>300</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="6">
+        <v>22338</v>
+      </c>
+      <c r="K7" s="6">
+        <v>63841</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="4">
+        <v>741540</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3975200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7">
+        <v>282.46140000000003</v>
+      </c>
+      <c r="C8" s="4">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4">
+        <v>100</v>
+      </c>
+      <c r="H8" s="5">
+        <v>300</v>
+      </c>
+      <c r="I8" s="4">
         <v>31509</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J8" s="6">
         <v>133847</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K8" s="6">
         <v>551470</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L8" s="6">
         <v>494928</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M8" s="4">
         <v>5345977</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N8" s="4">
         <v>19779576</v>
       </c>
     </row>
@@ -818,18 +906,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1056,14 +1144,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C9A587-8C95-48B5-A842-F4721C9A3A50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E757D89-FBD1-4745-9BBB-5EBBB2D8B99C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1076,6 +1156,14 @@
     <ds:schemaRef ds:uri="55a5d045-d387-40ca-ae81-7417199ee186"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C9A587-8C95-48B5-A842-F4721C9A3A50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>